<commit_message>
fixed time series update
</commit_message>
<xml_diff>
--- a/Model_setup/ISONE_data_file/Scenarios/Renewable_timeseries/Off_Shore_wind_ISO.xlsx
+++ b/Model_setup/ISONE_data_file/Scenarios/Renewable_timeseries/Off_Shore_wind_ISO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakdemi\Downloads\NREL_ISO_10_4_2021\NREL_ISO_9_24_2021\ISO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kakdemi\Documents\GitHub\ISONE_UCED_Sandy\Model_setup\ISONE_data_file\Scenarios\Renewable_timeseries\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="38400" windowHeight="20340" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="38400" windowHeight="20340"/>
   </bookViews>
   <sheets>
     <sheet name="All Zones Time Series - 2018" sheetId="4" r:id="rId1"/>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H384"/>
+  <dimension ref="A1:H385"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A365" workbookViewId="0">
+      <selection activeCell="B389" sqref="B389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10402,6 +10402,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A385" s="3">
+        <v>0</v>
+      </c>
+      <c r="B385" s="3">
+        <v>21.630223958333339</v>
+      </c>
+      <c r="C385" s="3">
+        <v>0</v>
+      </c>
+      <c r="D385" s="3">
+        <v>0</v>
+      </c>
+      <c r="E385" s="3">
+        <v>0</v>
+      </c>
+      <c r="F385" s="3">
+        <v>0</v>
+      </c>
+      <c r="G385" s="3">
+        <v>0</v>
+      </c>
+      <c r="H385" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10409,10 +10435,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H384"/>
+  <dimension ref="A1:H385"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView topLeftCell="A371" workbookViewId="0">
+      <selection activeCell="A390" sqref="A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20404,6 +20430,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A385" s="1">
+        <v>6388.3747656250016</v>
+      </c>
+      <c r="B385" s="1">
+        <v>1390.3012916666671</v>
+      </c>
+      <c r="C385" s="1">
+        <v>0</v>
+      </c>
+      <c r="D385" s="1">
+        <v>0</v>
+      </c>
+      <c r="E385" s="1">
+        <v>0</v>
+      </c>
+      <c r="F385" s="1">
+        <v>0</v>
+      </c>
+      <c r="G385" s="1">
+        <v>10920.27961979167</v>
+      </c>
+      <c r="H385" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20411,10 +20463,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H384"/>
+  <dimension ref="A1:H385"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A368" workbookViewId="0">
+      <selection activeCell="B389" sqref="B389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30406,6 +30458,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A385" s="1">
+        <v>15590.170385416672</v>
+      </c>
+      <c r="B385" s="1">
+        <v>3339.2590572916679</v>
+      </c>
+      <c r="C385" s="1">
+        <v>0</v>
+      </c>
+      <c r="D385" s="1">
+        <v>0</v>
+      </c>
+      <c r="E385" s="1">
+        <v>0</v>
+      </c>
+      <c r="F385" s="1">
+        <v>0</v>
+      </c>
+      <c r="G385" s="1">
+        <v>26649.927656250009</v>
+      </c>
+      <c r="H385" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>